<commit_message>
some changes in source code
</commit_message>
<xml_diff>
--- a/Test.xlsx
+++ b/Test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amsyar\Documents\cs230\part5\FYPSystem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AA1D045A-2B8F-444B-9669-B6F939E4B388}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{90447D51-3CFE-4769-ACDB-0CC403EAB710}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4860" yWindow="1920" windowWidth="21600" windowHeight="11385" xr2:uid="{F0B7C636-CCFF-43B3-856F-C7F7AEEE34A4}"/>
   </bookViews>
@@ -405,7 +405,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -425,16 +425,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>0.70256249024177841</v>
+        <v>0.93320580434120881</v>
       </c>
       <c r="B2">
-        <v>52388</v>
+        <v>41511</v>
       </c>
       <c r="C2">
-        <v>445</v>
+        <v>976</v>
       </c>
       <c r="D2">
-        <v>444</v>
+        <v>976</v>
       </c>
     </row>
   </sheetData>

</xml_diff>